<commit_message>
discharge and rearranging files
</commit_message>
<xml_diff>
--- a/Discharge/Gavi_02_2022-06-07_1110.xlsx
+++ b/Discharge/Gavi_02_2022-06-07_1110.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaylaemerson/Desktop/Ecuador2022/Discharge/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Discharge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4AA0622-9373-2242-B2B3-E72B5C72583A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C7D370-E78E-AB42-850C-1CC94CB62CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15780" xr2:uid="{1D37E556-BD7F-FA4F-A4F3-1DF81ED70988}"/>
+    <workbookView xWindow="-200" yWindow="2300" windowWidth="27640" windowHeight="15780" xr2:uid="{1D37E556-BD7F-FA4F-A4F3-1DF81ED70988}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -413,7 +415,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,9 +453,9 @@
       <c r="D2" s="1">
         <v>0.35</v>
       </c>
-      <c r="E2" s="1"/>
       <c r="F2" s="1">
-        <v>6.1999999999999998E-3</v>
+        <f>SUM(E2:E13)</f>
+        <v>6.0600000000000011E-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -469,8 +471,9 @@
       <c r="D3" s="1">
         <v>0.47499999999999998</v>
       </c>
-      <c r="E3" s="1">
-        <v>2.0000000000000001E-4</v>
+      <c r="E3">
+        <f>(D3-D2)*(B3/100)*C3</f>
+        <v>1.5749999999999998E-3</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -487,8 +490,9 @@
       <c r="D4" s="1">
         <v>0.625</v>
       </c>
-      <c r="E4" s="1">
-        <v>8.9999999999999998E-4</v>
+      <c r="E4">
+        <f>(D4-D3)*(B4/100)*C4</f>
+        <v>1.5000000000000005E-3</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -505,8 +509,9 @@
       <c r="D5" s="1">
         <v>0.77500000000000002</v>
       </c>
-      <c r="E5" s="1">
-        <v>4.7850000000000002E-3</v>
+      <c r="E5">
+        <f t="shared" ref="E4:E8" si="0">(D5-D4)*(B5/100)*C5</f>
+        <v>1.6200000000000001E-3</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -523,8 +528,9 @@
       <c r="D6" s="1">
         <v>0.92500000000000004</v>
       </c>
-      <c r="E6" s="1">
-        <v>2.4000000000000001E-4</v>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000003E-3</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -541,8 +547,9 @@
       <c r="D7" s="1">
         <v>1.075</v>
       </c>
-      <c r="E7" s="1">
-        <v>7.4999999999999993E-5</v>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1.6499999999999992E-4</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -559,7 +566,8 @@
       <c r="D8" s="1">
         <v>0.57499999999999996</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8" s="1"/>

</xml_diff>